<commit_message>
Project updated to use SUGAR v1
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -526,30 +526,12 @@
     <t>VALUE</t>
   </si>
   <si>
-    <t>GET_5_STARS</t>
-  </si>
-  <si>
     <t>GET_3_STARS_IN_ONE_GAME</t>
   </si>
   <si>
-    <t>PLAY_2_GAMES</t>
-  </si>
-  <si>
-    <t>ACCUMULATE_2_POINTS</t>
-  </si>
-  <si>
-    <t>Get 5 stars!</t>
-  </si>
-  <si>
     <t>Get 3 stars in one game!</t>
   </si>
   <si>
-    <t>Play 2 games!</t>
-  </si>
-  <si>
-    <t>Accumulate 2 points!</t>
-  </si>
-  <si>
     <t>FEEDBACK_MODE</t>
   </si>
   <si>
@@ -592,9 +574,6 @@
     <t>Game Locked!</t>
   </si>
   <si>
-    <t>Vergaar 2 punten!</t>
-  </si>
-  <si>
     <t>Fout: Niet in staat om prestaties op te halen</t>
   </si>
   <si>
@@ -622,16 +601,37 @@
     <t>Behaal 3 sterren in een spel!</t>
   </si>
   <si>
-    <t>Behaal 5 sterren!</t>
-  </si>
-  <si>
     <t>Meeste Sterren</t>
   </si>
   <si>
     <t>Er zijn geen achievements beschikbaar voor dit spel</t>
   </si>
   <si>
-    <t>Speel 2 spellen!</t>
+    <t>GET_25_STARS</t>
+  </si>
+  <si>
+    <t>Get 25 stars!</t>
+  </si>
+  <si>
+    <t>Behaal 25 sterren!</t>
+  </si>
+  <si>
+    <t>PLAY_15_GAMES</t>
+  </si>
+  <si>
+    <t>Play 15 games!</t>
+  </si>
+  <si>
+    <t>Speel 15 spellen!</t>
+  </si>
+  <si>
+    <t>ACCUMULATE_10000_POINTS</t>
+  </si>
+  <si>
+    <t>Accumulate 10000 points!</t>
+  </si>
+  <si>
+    <t>Vergaar 10000 punten!</t>
   </si>
 </sst>
 </file>
@@ -975,7 +975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -986,8 +986,8 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1020,13 +1020,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1037,7 +1037,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1125,7 +1125,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,46 +1229,46 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,46 +1284,46 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -1460,13 +1460,13 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1510,7 +1510,7 @@
         <v>138</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1581,13 +1581,13 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
provide an unlocked version of the game if launching not from url Dont send any data unless logged in to SUGAR
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Documents\Projects\RAGE\SpaceMods\Assets\Editor\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16440"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="210">
   <si>
     <t>Key</t>
   </si>
@@ -632,6 +637,21 @@
   </si>
   <si>
     <t>Vergaar 10000 punten!</t>
+  </si>
+  <si>
+    <t>PILOT_MODE_TITLE</t>
+  </si>
+  <si>
+    <t>PILOT_MODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SMI PILOT</t>
+  </si>
+  <si>
+    <t>Welcome to the pilot, press Play to start</t>
+  </si>
+  <si>
+    <t>Welcome to the pilot, press Play to continue</t>
   </si>
 </sst>
 </file>
@@ -643,12 +663,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -668,13 +682,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -686,25 +712,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -975,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -983,830 +1012,852 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
-    <col min="12" max="26" width="7.5703125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="15.140625" style="2"/>
+    <col min="1" max="1" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" style="1" customWidth="1"/>
+    <col min="12" max="26" width="7.54296875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="15.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C30" s="4" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="31" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="33" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="35" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="36" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="37" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="39" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C39" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="40" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="42" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C42" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+    <row r="43" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+    <row r="44" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C44" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="45" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="46" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    <row r="47" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="48" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="49" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="50" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+    <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+    <row r="53" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="54" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C54" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+    <row r="55" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+    <row r="56" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C56" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+    <row r="58" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C58" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+    <row r="59" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C59" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+    <row r="60" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C60" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+    <row r="61" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+    <row r="62" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+    <row r="63" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C63" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+    <row r="64" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+    <row r="65" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+    <row r="66" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C66" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+    <row r="67" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C67" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+    <row r="68" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C68" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="69" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C69" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+    <row r="70" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C70" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+    <row r="71" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+    <row r="72" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C72" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="73" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C73" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="74" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C74" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add session expired text for when the time stamp is no longer valid Add check for isPilot, so that the game will only ever be locked during the pilot
AWAITING TRANSLATIONS FROM ROB
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="213">
   <si>
     <t>Key</t>
   </si>
@@ -645,13 +645,22 @@
     <t>PILOT_MODE_DESCRIPTION</t>
   </si>
   <si>
-    <t>SMI PILOT</t>
-  </si>
-  <si>
-    <t>Welcome to the pilot, press Play to start</t>
-  </si>
-  <si>
     <t>Welcome to the pilot, press Play to continue</t>
+  </si>
+  <si>
+    <t>PILOT_MODE_EXPIRED_TITLE</t>
+  </si>
+  <si>
+    <t>Session Expired</t>
+  </si>
+  <si>
+    <t>SMI Pilot</t>
+  </si>
+  <si>
+    <t>PILOT_MODE_EXPIRED_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Pilot session no longer valid</t>
   </si>
 </sst>
 </file>
@@ -1012,16 +1021,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="59" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.453125" style="1" customWidth="1"/>
@@ -1335,529 +1344,551 @@
     </row>
     <row r="28" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>205</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>193</v>
+        <v>210</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>51</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+    <row r="37" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+    <row r="38" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>135</v>
+      <c r="A42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>180</v>
+      <c r="A44" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>122</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>118</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>152</v>
+      <c r="A61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="65" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+    <row r="66" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+    <row r="67" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>160</v>
+      <c r="A69" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>103</v>
+      <c r="A71" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="s">
+    <row r="75" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
+    <row r="76" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add ambiguous error code for not logged in to not confuse, no login button so "not logged in" is confusing
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -471,9 +471,6 @@
     <t>NO_USER_ERROR</t>
   </si>
   <si>
-    <t>Error: No user currently signed in.</t>
-  </si>
-  <si>
     <t>Fout: Geen gebruiker die momenteel is aangemeld</t>
   </si>
   <si>
@@ -661,6 +658,9 @@
   </si>
   <si>
     <t>Pilot session no longer valid</t>
+  </si>
+  <si>
+    <t>Error: 'Low Fuel'.\nUnable to get data.</t>
   </si>
 </sst>
 </file>
@@ -1025,7 +1025,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1058,13 +1058,13 @@
     </row>
     <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1075,7 +1075,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1163,7 +1163,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1267,46 +1267,46 @@
     </row>
     <row r="21" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1322,90 +1322,90 @@
     </row>
     <row r="26" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C31" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.35">
@@ -1542,13 +1542,13 @@
     </row>
     <row r="46" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>138</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1633,10 +1633,10 @@
         <v>148</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1663,13 +1663,13 @@
     </row>
     <row r="57" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1729,13 +1729,13 @@
     </row>
     <row r="63" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1762,24 +1762,24 @@
     </row>
     <row r="66" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1817,13 +1817,13 @@
     </row>
     <row r="71" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1861,29 +1861,29 @@
     </row>
     <row r="75" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Add dutch translation for pilot mode and session expired
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="216">
   <si>
     <t>Key</t>
   </si>
@@ -661,6 +661,15 @@
   </si>
   <si>
     <t>Error: 'Low Fuel'.\nUnable to get data.</t>
+  </si>
+  <si>
+    <t>Sessie Verlopen</t>
+  </si>
+  <si>
+    <t>Pilot sessie is niet langer geldig</t>
+  </si>
+  <si>
+    <t>Welkom bij de pilot, klik op Speel om door te gaan</t>
   </si>
 </sst>
 </file>
@@ -693,23 +702,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -721,9 +724,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -737,12 +739,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1021,11 +1020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1349,8 +1348,8 @@
       <c r="B28" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>208</v>
+      <c r="C28" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1360,8 +1359,8 @@
       <c r="B29" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>211</v>
+      <c r="C29" s="4" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1371,7 +1370,7 @@
       <c r="B30" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>209</v>
       </c>
     </row>
@@ -1383,7 +1382,7 @@
         <v>206</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1397,7 +1396,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>195</v>
       </c>
@@ -1408,7 +1407,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
@@ -1418,8 +1417,9 @@
       <c r="C34" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>55</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>129</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>132</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>134</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>177</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>74</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Update names of feedback modes to be less confusing
</commit_message>
<xml_diff>
--- a/Assets/Editor/Localization/SMILocalization.xlsx
+++ b/Assets/Editor/Localization/SMILocalization.xlsx
@@ -537,18 +537,12 @@
     <t>FEEDBACK_MODE</t>
   </si>
   <si>
-    <t>FEEDBACK_MINIMAL</t>
-  </si>
-  <si>
     <t>FEEDBACK_INGAME</t>
   </si>
   <si>
     <t>FEEDBACK_ENDGAME</t>
   </si>
   <si>
-    <t>Minimal</t>
-  </si>
-  <si>
     <t>In Game</t>
   </si>
   <si>
@@ -588,9 +582,6 @@
     <t>Bezig in Spel</t>
   </si>
   <si>
-    <t>Minimaal</t>
-  </si>
-  <si>
     <t>Terugkoppeling Modus</t>
   </si>
   <si>
@@ -670,6 +661,15 @@
   </si>
   <si>
     <t>Welkom bij de pilot, klik op Speel om door te gaan</t>
+  </si>
+  <si>
+    <t>FEEDBACK_INREVIEW</t>
+  </si>
+  <si>
+    <t>In Review</t>
+  </si>
+  <si>
+    <t>In beoordeling</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1024,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1057,13 +1057,13 @@
     </row>
     <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1162,7 +1162,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1266,35 +1266,35 @@
     </row>
     <row r="21" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>174</v>
+        <v>214</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1302,10 +1302,10 @@
         <v>170</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1321,68 +1321,68 @@
     </row>
     <row r="26" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1393,18 +1393,18 @@
         <v>169</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.35">
@@ -1542,13 +1542,13 @@
     </row>
     <row r="46" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="C46" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>138</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
@@ -1633,7 +1633,7 @@
         <v>148</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>149</v>
@@ -1663,13 +1663,13 @@
     </row>
     <row r="57" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">

</xml_diff>